<commit_message>
upload an initial segmentation dnn model.
</commit_message>
<xml_diff>
--- a/labelme/name_list_with_pixel_value.xlsx
+++ b/labelme/name_list_with_pixel_value.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylee\Documents\alphado\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE824CE4-F9D5-42DF-B102-52E017795D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20850" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Third_eyelid_protrude</t>
   </si>
@@ -63,18 +57,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>keratoconjunctivitis_sicca_pigmen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>keratoconjunctivitis_sicca_flare</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>keratoconjunctivitis_sicca_cornea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>uveitis_discoloration</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -143,18 +129,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>conceal_pus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cornceal_scratch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cornceal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>gataract</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -189,13 +163,43 @@
   <si>
     <t>pixelValue</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corneal_degeneration_Glass_fiber</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>corneal_degeneration_opacity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ectropion_corneal_damage</t>
+  </si>
+  <si>
+    <t>keratoconjunctivitis_sicca_pigmentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corneal_pus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corneal_scratch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corneal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>keratoconjunctivitis_sicca_corneal_opacity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +211,13 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -231,8 +242,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -293,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -328,7 +342,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -505,34 +519,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.125" customWidth="1"/>
+    <col min="1" max="1" width="36.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -540,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -548,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -556,7 +570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -564,7 +578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -572,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -580,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -588,71 +602,71 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -660,180 +674,204 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B39">
         <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="1">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>